<commit_message>
Changes to CO2 balancers:
CaCO3 calcination does not have to be 100%
sinter plant iron oxidation CO2 assumed counted in combustion
</commit_message>
<xml_diff>
--- a/data/steel/steel_IEAGHG_var.xlsx
+++ b/data/steel/steel_IEAGHG_var.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C42E3C-FC19-F348-B78E-49916E4E551C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9405" yWindow="555" windowWidth="17445" windowHeight="16185" activeTab="2"/>
+    <workbookView xWindow="3100" yWindow="560" windowWidth="23380" windowHeight="16180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke Oven" sheetId="2" r:id="rId1"/>
@@ -20,17 +21,17 @@
     <sheet name="Forming" sheetId="13" r:id="rId6"/>
     <sheet name="Reference Values" sheetId="14" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Tanzer - TBM</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -101,13 +102,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samantha Tanzer - TBM</author>
     <author>S.E. Tanzer</author>
   </authors>
   <commentList>
-    <comment ref="J5" authorId="0" shapeId="0">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -140,28 +141,56 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>S.E. Tanzer:</t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-this is supplementary natural gas demand only.
-Heat export should be 1.6742 GJ</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">this is supplementary natural gas demand only.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Heat export should be 1.6742 GJ</t>
         </r>
       </text>
     </comment>
@@ -170,12 +199,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -208,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -274,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -312,12 +341,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -351,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -384,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -457,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -548,7 +577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -639,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -677,7 +706,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
   <si>
     <t>Electricity Demand</t>
   </si>
@@ -721,9 +750,6 @@
     <t>Scrap Fraction of Steel</t>
   </si>
   <si>
-    <t>IEAGHG 2013</t>
-  </si>
-  <si>
     <t>mj biomass / mj energy use</t>
   </si>
   <si>
@@ -1025,17 +1051,27 @@
   </si>
   <si>
     <t>O2 demand</t>
+  </si>
+  <si>
+    <t>ieaghg-reference</t>
+  </si>
+  <si>
+    <t>CO2 not calcinated</t>
+  </si>
+  <si>
+    <t>% CO2 in CaCO3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,19 +1163,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1242,7 +1265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1290,6 +1313,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1383,6 +1407,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1418,6 +1459,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1593,29 +1651,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -1627,31 +1685,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1660,7 +1718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1685,19 +1743,19 @@
         <v>charcoal</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <f>1/1.2852</f>
         <v>0.77808901338313108</v>
       </c>
       <c r="D5">
-        <f>35*3.6/1000</f>
+        <f>35*'Reference Values'!B18</f>
         <v>0.126</v>
       </c>
       <c r="E5">
@@ -1708,7 +1766,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1719,25 +1777,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1745,19 +1803,19 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1766,45 +1824,45 @@
         <v>0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
       <c r="I2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2"/>
       <c r="F3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1845,9 +1903,9 @@
         <v>0.69769999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>9.4E-2</v>
@@ -1866,14 +1924,14 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <f>'Reference Values'!F4*4.2/1000</f>
         <v>7.2786000000000003E-2</v>
       </c>
       <c r="I5">
-        <f>32*3.6/1000</f>
+        <f>32*'Reference Values'!B18</f>
         <v>0.1152</v>
       </c>
       <c r="J5">
@@ -1886,48 +1944,50 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="6" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
       </c>
       <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
@@ -1939,19 +1999,22 @@
         <v>0</v>
       </c>
       <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
-        <v>40</v>
-      </c>
       <c r="N1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="P1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1965,7 +2028,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1974,30 +2037,33 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
         <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
       </c>
       <c r="N2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2053,13 +2119,17 @@
         <f t="shared" si="0"/>
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="45">
+        <f>O5</f>
+        <v>7.0422535211267609E-2</v>
+      </c>
+      <c r="P4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>0.95</v>
@@ -2077,7 +2147,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <f>0.1253+0.3518</f>
@@ -2103,13 +2173,17 @@
       <c r="N5">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="45">
+        <f>3/42.6</f>
+        <v>7.0422535211267609E-2</v>
+      </c>
+      <c r="P5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6">
         <v>0.95</v>
@@ -2127,7 +2201,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <f>0.1253+0.3526</f>
@@ -2153,7 +2227,11 @@
       <c r="N6">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="45">
+        <f>O5</f>
+        <v>7.0422535211267609E-2</v>
+      </c>
+      <c r="P6">
         <v>9.4799999999999995E-2</v>
       </c>
     </row>
@@ -2165,30 +2243,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -2200,54 +2278,54 @@
         <v>0</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
         <v>51</v>
       </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" t="s">
-        <v>52</v>
-      </c>
       <c r="I2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2284,9 +2362,9 @@
         <v>7.4236530739716242E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <f>((900.8+116.9+73.1+5)-1000)/(900.8+116.9+73.1+5)</f>
@@ -2327,36 +2405,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
@@ -2365,47 +2443,47 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>59</v>
       </c>
-      <c r="I2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
@@ -2415,7 +2493,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -2452,9 +2530,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>0.01</v>
@@ -2490,24 +2568,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -2516,32 +2594,32 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
         <v>112</v>
       </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
       <c r="E2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2562,9 +2640,9 @@
         <v>6.8657369929508343E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <f>((1086.3-1052.6)+(1052.6-1000))/1000</f>
@@ -2590,72 +2668,72 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
       <c r="B3" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="39">
         <v>12</v>
@@ -2665,7 +2743,7 @@
         <v>5.3537967341839917E-4</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="19">
         <v>17.329999999999998</v>
@@ -2683,12 +2761,12 @@
         <v>34.468724082518165</v>
       </c>
       <c r="J4" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="39">
         <v>16.042459999999998</v>
@@ -2698,7 +2776,7 @@
         <v>7.1573391630231102E-4</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="19">
         <v>3.2</v>
@@ -2716,12 +2794,12 @@
         <v>2.3682220828775362</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="39">
         <v>28.010100000000001</v>
@@ -2731,7 +2809,7 @@
         <v>1.2496698492013921E-3</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="19">
         <v>7.47</v>
@@ -2749,12 +2827,12 @@
         <v>3.9112454453016037</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="39">
         <v>44.009500000000003</v>
@@ -2764,7 +2842,7 @@
         <v>1.963482644775587E-3</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="27"/>
@@ -2776,12 +2854,12 @@
         <v>2.77</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="39">
         <v>2.0158800000000001</v>
@@ -2795,9 +2873,9 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="39">
         <v>18.015280000000001</v>
@@ -2807,15 +2885,15 @@
         <v>8.0375122691175155E-4</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="39">
         <f>(78.12+92.15+106.7)/3</f>
@@ -2827,18 +2905,18 @@
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="39">
         <v>28.013400000000001</v>
@@ -2848,7 +2926,7 @@
         <v>1.2498170786115822E-3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11" s="12">
         <v>0.57879999999999998</v>
@@ -2858,9 +2936,9 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="39">
         <v>31.998799999999999</v>
@@ -2870,7 +2948,7 @@
         <v>1.4276255911483892E-3</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="12">
         <v>0.94240000000000002</v>
@@ -2880,12 +2958,12 @@
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="42"/>
       <c r="C13" s="31"/>
       <c r="E13" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F13" s="12">
         <v>0.99909999999999999</v>
@@ -2895,11 +2973,11 @@
       </c>
       <c r="H13" s="11"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="E14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="12">
         <v>0.98729999999999996</v>
@@ -2909,14 +2987,14 @@
       </c>
       <c r="H14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="E15" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -2924,25 +3002,25 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="17"/>
       <c r="B16" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="C16" s="40"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="B17" s="30">
         <v>3.6</v>
       </c>
       <c r="C17" s="39"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18" s="29">
         <f>B17/1000</f>
@@ -2950,9 +3028,9 @@
       </c>
       <c r="C18" s="39"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="31">
         <f>1/0.022414</f>

</xml_diff>